<commit_message>
updated order for plotting
</commit_message>
<xml_diff>
--- a/weight_estimation/WTO_vs_WS_turboprop_profile1.xlsx
+++ b/weight_estimation/WTO_vs_WS_turboprop_profile1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\GitHub\443_design_problem\weight_estimation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A2F2AF2-4BAB-4118-8673-7C1694362D9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11A10BC-F2FA-4384-9699-30C7633F64A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{668FAD8C-68CB-4080-8947-0AEE8F465407}"/>
   </bookViews>
@@ -404,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87263ECD-7D18-435B-8944-4232101EC974}">
   <dimension ref="A1:H71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>